<commit_message>
Planteo de clase Incorporacion
Co-Authored-By: Pablo1864 <130506261+Pablo1864@users.noreply.github.com>
Co-Authored-By: Maryolivera <128436041+Maryolivera@users.noreply.github.com>
Co-Authored-By: alex-astudillo <105954347+ast-alex@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Metodos ( relaciones con la tabla ).xlsx
+++ b/Metodos ( relaciones con la tabla ).xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="62">
   <si>
     <t>Dni</t>
   </si>
@@ -566,12 +566,42 @@
   <si>
     <t>4°</t>
   </si>
+  <si>
+    <t>EQUIPO              ↓</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MIEMBRO      ↓ </t>
+  </si>
+  <si>
+    <t>ID EQUIPO</t>
+  </si>
+  <si>
+    <t>NOMBRE EQUIPO</t>
+  </si>
+  <si>
+    <t>NOMBRE PROYECTO</t>
+  </si>
+  <si>
+    <t>FECHA CREACION</t>
+  </si>
+  <si>
+    <t>ESTADO</t>
+  </si>
+  <si>
+    <t>NOMBRE Y APELLIDO</t>
+  </si>
+  <si>
+    <t>DNI</t>
+  </si>
+  <si>
+    <t>FECHA INCORPORACION</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="16">
+  <fonts count="17">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -689,6 +719,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="28"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="17">
     <fill>
@@ -788,7 +825,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="55">
+  <borders count="57">
     <border>
       <left/>
       <right/>
@@ -1466,11 +1503,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="293">
+  <cellXfs count="305">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1556,6 +1619,519 @@
     <xf numFmtId="0" fontId="10" fillId="6" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1574,9 +2150,6 @@
     <xf numFmtId="0" fontId="13" fillId="15" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="7" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1620,9 +2193,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1793,530 +2363,57 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2614,8 +2711,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:W66"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31:W66"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2655,29 +2752,29 @@
       <c r="A2" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="266" t="s">
+      <c r="B2" s="91" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="267"/>
-      <c r="D2" s="270" t="s">
+      <c r="C2" s="92"/>
+      <c r="D2" s="95" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="271"/>
+      <c r="E2" s="96"/>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
       <c r="H2" s="7"/>
       <c r="J2" s="5"/>
-      <c r="K2" s="258" t="s">
+      <c r="K2" s="83" t="s">
         <v>23</v>
       </c>
-      <c r="L2" s="259"/>
-      <c r="M2" s="260"/>
+      <c r="L2" s="84"/>
+      <c r="M2" s="85"/>
       <c r="N2" s="6"/>
-      <c r="O2" s="220" t="s">
+      <c r="O2" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="P2" s="221"/>
-      <c r="Q2" s="222"/>
+      <c r="P2" s="46"/>
+      <c r="Q2" s="47"/>
       <c r="R2" s="18"/>
       <c r="S2" s="18"/>
       <c r="T2" s="18"/>
@@ -2689,21 +2786,21 @@
       <c r="A3" s="15">
         <v>6</v>
       </c>
-      <c r="B3" s="268"/>
-      <c r="C3" s="269"/>
-      <c r="D3" s="272"/>
-      <c r="E3" s="273"/>
+      <c r="B3" s="93"/>
+      <c r="C3" s="94"/>
+      <c r="D3" s="97"/>
+      <c r="E3" s="98"/>
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
       <c r="H3" s="7"/>
       <c r="J3" s="5"/>
-      <c r="K3" s="261"/>
-      <c r="L3" s="262"/>
-      <c r="M3" s="263"/>
+      <c r="K3" s="86"/>
+      <c r="L3" s="87"/>
+      <c r="M3" s="88"/>
       <c r="N3" s="6"/>
-      <c r="O3" s="223"/>
-      <c r="P3" s="224"/>
-      <c r="Q3" s="225"/>
+      <c r="O3" s="48"/>
+      <c r="P3" s="49"/>
+      <c r="Q3" s="50"/>
       <c r="R3" s="6"/>
       <c r="S3" s="6"/>
       <c r="T3" s="6"/>
@@ -2744,20 +2841,20 @@
       <c r="G5" s="6"/>
       <c r="H5" s="7"/>
       <c r="J5" s="5"/>
-      <c r="K5" s="285" t="s">
+      <c r="K5" s="112" t="s">
         <v>34</v>
       </c>
-      <c r="L5" s="286"/>
-      <c r="M5" s="286"/>
-      <c r="N5" s="287"/>
-      <c r="O5" s="287"/>
-      <c r="P5" s="287"/>
-      <c r="Q5" s="287"/>
-      <c r="R5" s="287"/>
-      <c r="S5" s="287"/>
-      <c r="T5" s="287"/>
-      <c r="U5" s="287"/>
-      <c r="V5" s="288"/>
+      <c r="L5" s="113"/>
+      <c r="M5" s="113"/>
+      <c r="N5" s="114"/>
+      <c r="O5" s="114"/>
+      <c r="P5" s="114"/>
+      <c r="Q5" s="114"/>
+      <c r="R5" s="114"/>
+      <c r="S5" s="114"/>
+      <c r="T5" s="114"/>
+      <c r="U5" s="114"/>
+      <c r="V5" s="115"/>
       <c r="W5" s="7"/>
     </row>
     <row r="6" spans="1:23" ht="21.75" thickBot="1">
@@ -2772,25 +2869,25 @@
       <c r="G6" s="6"/>
       <c r="H6" s="7"/>
       <c r="J6" s="5"/>
-      <c r="K6" s="289" t="s">
+      <c r="K6" s="116" t="s">
         <v>2</v>
       </c>
-      <c r="L6" s="290"/>
+      <c r="L6" s="117"/>
       <c r="M6" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="N6" s="264" t="s">
+      <c r="N6" s="89" t="s">
         <v>31</v>
       </c>
-      <c r="O6" s="265"/>
-      <c r="P6" s="216" t="s">
+      <c r="O6" s="90"/>
+      <c r="P6" s="41" t="s">
         <v>30</v>
       </c>
-      <c r="Q6" s="217"/>
-      <c r="R6" s="214" t="s">
+      <c r="Q6" s="42"/>
+      <c r="R6" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="S6" s="215"/>
+      <c r="S6" s="40"/>
       <c r="T6" s="37" t="s">
         <v>2</v>
       </c>
@@ -2812,25 +2909,25 @@
       <c r="G7" s="6"/>
       <c r="H7" s="7"/>
       <c r="J7" s="5"/>
-      <c r="K7" s="191" t="s">
+      <c r="K7" s="134" t="s">
         <v>22</v>
       </c>
-      <c r="L7" s="192"/>
-      <c r="M7" s="195">
+      <c r="L7" s="135"/>
+      <c r="M7" s="136">
         <v>1</v>
       </c>
-      <c r="N7" s="118">
+      <c r="N7" s="155">
         <v>2</v>
       </c>
-      <c r="O7" s="119"/>
-      <c r="P7" s="256">
+      <c r="O7" s="138"/>
+      <c r="P7" s="81">
         <v>13</v>
       </c>
-      <c r="Q7" s="257"/>
-      <c r="R7" s="189">
+      <c r="Q7" s="82"/>
+      <c r="R7" s="132">
         <v>1</v>
       </c>
-      <c r="S7" s="190"/>
+      <c r="S7" s="133"/>
       <c r="T7" s="35" t="s">
         <v>32</v>
       </c>
@@ -2852,15 +2949,15 @@
       <c r="G8" s="6"/>
       <c r="H8" s="7"/>
       <c r="J8" s="5"/>
-      <c r="K8" s="191"/>
-      <c r="L8" s="192"/>
-      <c r="M8" s="195"/>
-      <c r="N8" s="120"/>
-      <c r="O8" s="121"/>
-      <c r="P8" s="187"/>
-      <c r="Q8" s="188"/>
-      <c r="R8" s="208"/>
-      <c r="S8" s="209"/>
+      <c r="K8" s="134"/>
+      <c r="L8" s="135"/>
+      <c r="M8" s="136"/>
+      <c r="N8" s="118"/>
+      <c r="O8" s="204"/>
+      <c r="P8" s="128"/>
+      <c r="Q8" s="129"/>
+      <c r="R8" s="149"/>
+      <c r="S8" s="150"/>
       <c r="T8" s="30"/>
       <c r="U8" s="30"/>
       <c r="V8" s="31"/>
@@ -2890,15 +2987,15 @@
       </c>
       <c r="H9" s="7"/>
       <c r="J9" s="5"/>
-      <c r="K9" s="191"/>
-      <c r="L9" s="192"/>
-      <c r="M9" s="195"/>
-      <c r="N9" s="120"/>
-      <c r="O9" s="121"/>
-      <c r="P9" s="187"/>
-      <c r="Q9" s="188"/>
-      <c r="R9" s="208"/>
-      <c r="S9" s="209"/>
+      <c r="K9" s="134"/>
+      <c r="L9" s="135"/>
+      <c r="M9" s="136"/>
+      <c r="N9" s="118"/>
+      <c r="O9" s="204"/>
+      <c r="P9" s="128"/>
+      <c r="Q9" s="129"/>
+      <c r="R9" s="149"/>
+      <c r="S9" s="150"/>
       <c r="T9" s="30"/>
       <c r="U9" s="30"/>
       <c r="V9" s="31"/>
@@ -2928,15 +3025,15 @@
       </c>
       <c r="H10" s="7"/>
       <c r="J10" s="5"/>
-      <c r="K10" s="193"/>
-      <c r="L10" s="194"/>
-      <c r="M10" s="185"/>
-      <c r="N10" s="122"/>
-      <c r="O10" s="123"/>
-      <c r="P10" s="204"/>
-      <c r="Q10" s="205"/>
-      <c r="R10" s="210"/>
-      <c r="S10" s="211"/>
+      <c r="K10" s="104"/>
+      <c r="L10" s="105"/>
+      <c r="M10" s="125"/>
+      <c r="N10" s="205"/>
+      <c r="O10" s="124"/>
+      <c r="P10" s="145"/>
+      <c r="Q10" s="146"/>
+      <c r="R10" s="151"/>
+      <c r="S10" s="152"/>
       <c r="T10" s="32"/>
       <c r="U10" s="32"/>
       <c r="V10" s="33"/>
@@ -2966,25 +3063,25 @@
       </c>
       <c r="H11" s="7"/>
       <c r="J11" s="5"/>
-      <c r="K11" s="197" t="s">
+      <c r="K11" s="139" t="s">
         <v>24</v>
       </c>
-      <c r="L11" s="198"/>
-      <c r="M11" s="196">
+      <c r="L11" s="140"/>
+      <c r="M11" s="137">
         <v>1</v>
       </c>
-      <c r="N11" s="124">
+      <c r="N11" s="206">
         <v>6</v>
       </c>
-      <c r="O11" s="125"/>
-      <c r="P11" s="206">
+      <c r="O11" s="207"/>
+      <c r="P11" s="147">
         <v>17</v>
       </c>
-      <c r="Q11" s="207"/>
-      <c r="R11" s="212">
+      <c r="Q11" s="148"/>
+      <c r="R11" s="153">
         <v>5</v>
       </c>
-      <c r="S11" s="213"/>
+      <c r="S11" s="154"/>
       <c r="T11" s="28" t="s">
         <v>7</v>
       </c>
@@ -3006,15 +3103,15 @@
       <c r="G12" s="6"/>
       <c r="H12" s="7"/>
       <c r="J12" s="5"/>
-      <c r="K12" s="199"/>
-      <c r="L12" s="200"/>
-      <c r="M12" s="119"/>
-      <c r="N12" s="120"/>
-      <c r="O12" s="121"/>
-      <c r="P12" s="187"/>
-      <c r="Q12" s="188"/>
-      <c r="R12" s="201"/>
-      <c r="S12" s="202"/>
+      <c r="K12" s="141"/>
+      <c r="L12" s="142"/>
+      <c r="M12" s="138"/>
+      <c r="N12" s="118"/>
+      <c r="O12" s="204"/>
+      <c r="P12" s="128"/>
+      <c r="Q12" s="129"/>
+      <c r="R12" s="143"/>
+      <c r="S12" s="144"/>
       <c r="T12" s="30"/>
       <c r="U12" s="30"/>
       <c r="V12" s="31"/>
@@ -3022,35 +3119,35 @@
     </row>
     <row r="13" spans="1:23" ht="20.25" customHeight="1" thickBot="1">
       <c r="A13" s="5"/>
-      <c r="B13" s="274" t="s">
+      <c r="B13" s="99" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="275"/>
-      <c r="D13" s="275"/>
-      <c r="E13" s="275"/>
-      <c r="F13" s="276"/>
+      <c r="C13" s="100"/>
+      <c r="D13" s="100"/>
+      <c r="E13" s="100"/>
+      <c r="F13" s="101"/>
       <c r="G13" s="13" t="s">
         <v>4</v>
       </c>
       <c r="H13" s="7"/>
       <c r="J13" s="5"/>
-      <c r="K13" s="277" t="s">
+      <c r="K13" s="102" t="s">
         <v>25</v>
       </c>
-      <c r="L13" s="278"/>
-      <c r="M13" s="123">
+      <c r="L13" s="103"/>
+      <c r="M13" s="124">
         <v>1</v>
       </c>
-      <c r="N13" s="120"/>
-      <c r="O13" s="121"/>
-      <c r="P13" s="187">
+      <c r="N13" s="118"/>
+      <c r="O13" s="204"/>
+      <c r="P13" s="128">
         <v>18</v>
       </c>
-      <c r="Q13" s="188"/>
-      <c r="R13" s="201">
+      <c r="Q13" s="129"/>
+      <c r="R13" s="143">
         <v>6</v>
       </c>
-      <c r="S13" s="202"/>
+      <c r="S13" s="144"/>
       <c r="T13" s="30" t="s">
         <v>8</v>
       </c>
@@ -3063,10 +3160,10 @@
       <c r="W13" s="7"/>
     </row>
     <row r="14" spans="1:23" ht="20.25" customHeight="1" thickBot="1">
-      <c r="A14" s="218" t="s">
+      <c r="A14" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="219"/>
+      <c r="B14" s="44"/>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
@@ -3074,15 +3171,15 @@
       <c r="G14" s="6"/>
       <c r="H14" s="7"/>
       <c r="J14" s="5"/>
-      <c r="K14" s="193"/>
-      <c r="L14" s="194"/>
-      <c r="M14" s="185"/>
-      <c r="N14" s="126"/>
-      <c r="O14" s="127"/>
-      <c r="P14" s="172"/>
-      <c r="Q14" s="173"/>
-      <c r="R14" s="126"/>
-      <c r="S14" s="203"/>
+      <c r="K14" s="104"/>
+      <c r="L14" s="105"/>
+      <c r="M14" s="125"/>
+      <c r="N14" s="120"/>
+      <c r="O14" s="208"/>
+      <c r="P14" s="130"/>
+      <c r="Q14" s="131"/>
+      <c r="R14" s="120"/>
+      <c r="S14" s="121"/>
       <c r="T14" s="25"/>
       <c r="U14" s="25"/>
       <c r="V14" s="26"/>
@@ -3098,14 +3195,14 @@
       <c r="G15" s="6"/>
       <c r="H15" s="7"/>
       <c r="J15" s="5"/>
-      <c r="K15" s="232"/>
-      <c r="L15" s="233"/>
-      <c r="M15" s="186"/>
-      <c r="N15" s="128"/>
-      <c r="O15" s="129"/>
-      <c r="P15" s="291"/>
-      <c r="Q15" s="292"/>
-      <c r="R15" s="118"/>
+      <c r="K15" s="57"/>
+      <c r="L15" s="58"/>
+      <c r="M15" s="126"/>
+      <c r="N15" s="209"/>
+      <c r="O15" s="127"/>
+      <c r="P15" s="122"/>
+      <c r="Q15" s="123"/>
+      <c r="R15" s="155"/>
       <c r="S15" s="156"/>
       <c r="T15" s="23"/>
       <c r="U15" s="23"/>
@@ -3122,53 +3219,73 @@
       <c r="G16" s="9"/>
       <c r="H16" s="10"/>
       <c r="J16" s="5"/>
-      <c r="K16" s="234"/>
-      <c r="L16" s="235"/>
-      <c r="M16" s="129"/>
-      <c r="N16" s="130"/>
-      <c r="O16" s="131"/>
-      <c r="P16" s="183"/>
-      <c r="Q16" s="184"/>
-      <c r="R16" s="120"/>
-      <c r="S16" s="157"/>
+      <c r="K16" s="59"/>
+      <c r="L16" s="60"/>
+      <c r="M16" s="127"/>
+      <c r="N16" s="173"/>
+      <c r="O16" s="174"/>
+      <c r="P16" s="171"/>
+      <c r="Q16" s="172"/>
+      <c r="R16" s="118"/>
+      <c r="S16" s="119"/>
       <c r="T16" s="11"/>
       <c r="U16" s="11"/>
       <c r="V16" s="24"/>
       <c r="W16" s="7"/>
     </row>
-    <row r="17" spans="10:23" ht="20.25" customHeight="1">
+    <row r="17" spans="1:23" ht="20.25" customHeight="1" thickBot="1">
       <c r="J17" s="5"/>
-      <c r="K17" s="236"/>
-      <c r="L17" s="237"/>
-      <c r="M17" s="170"/>
-      <c r="N17" s="130"/>
-      <c r="O17" s="131"/>
-      <c r="P17" s="183"/>
-      <c r="Q17" s="184"/>
-      <c r="R17" s="120"/>
-      <c r="S17" s="157"/>
+      <c r="K17" s="61"/>
+      <c r="L17" s="62"/>
+      <c r="M17" s="169"/>
+      <c r="N17" s="173"/>
+      <c r="O17" s="174"/>
+      <c r="P17" s="171"/>
+      <c r="Q17" s="172"/>
+      <c r="R17" s="118"/>
+      <c r="S17" s="119"/>
       <c r="T17" s="11"/>
       <c r="U17" s="11"/>
       <c r="V17" s="24"/>
       <c r="W17" s="7"/>
     </row>
-    <row r="18" spans="10:23" ht="20.25" customHeight="1" thickBot="1">
+    <row r="18" spans="1:23" ht="20.25" customHeight="1" thickBot="1">
+      <c r="A18" s="2"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="4"/>
       <c r="J18" s="5"/>
-      <c r="K18" s="238"/>
-      <c r="L18" s="239"/>
-      <c r="M18" s="171"/>
-      <c r="N18" s="132"/>
-      <c r="O18" s="133"/>
-      <c r="P18" s="172"/>
-      <c r="Q18" s="173"/>
-      <c r="R18" s="126"/>
-      <c r="S18" s="203"/>
+      <c r="K18" s="63"/>
+      <c r="L18" s="64"/>
+      <c r="M18" s="170"/>
+      <c r="N18" s="175"/>
+      <c r="O18" s="176"/>
+      <c r="P18" s="130"/>
+      <c r="Q18" s="131"/>
+      <c r="R18" s="120"/>
+      <c r="S18" s="121"/>
       <c r="T18" s="25"/>
       <c r="U18" s="25"/>
       <c r="V18" s="26"/>
       <c r="W18" s="7"/>
     </row>
-    <row r="19" spans="10:23" ht="29.25" customHeight="1" thickBot="1">
+    <row r="19" spans="1:23" ht="29.25" customHeight="1" thickBot="1">
+      <c r="A19" s="5"/>
+      <c r="B19" s="297" t="s">
+        <v>53</v>
+      </c>
+      <c r="C19" s="298"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="291" t="s">
+        <v>52</v>
+      </c>
+      <c r="F19" s="292"/>
+      <c r="G19" s="293"/>
+      <c r="H19" s="7"/>
       <c r="J19" s="5"/>
       <c r="K19" s="6"/>
       <c r="L19" s="6"/>
@@ -3184,81 +3301,131 @@
       <c r="V19" s="6"/>
       <c r="W19" s="7"/>
     </row>
-    <row r="20" spans="10:23">
+    <row r="20" spans="1:23" ht="15.75" thickBot="1">
+      <c r="A20" s="5"/>
+      <c r="B20" s="299"/>
+      <c r="C20" s="300"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="294"/>
+      <c r="F20" s="295"/>
+      <c r="G20" s="296"/>
+      <c r="H20" s="7"/>
       <c r="J20" s="5"/>
       <c r="K20" s="6"/>
-      <c r="L20" s="244" t="s">
+      <c r="L20" s="69" t="s">
         <v>29</v>
       </c>
-      <c r="M20" s="245"/>
-      <c r="N20" s="248" t="s">
+      <c r="M20" s="70"/>
+      <c r="N20" s="73" t="s">
         <v>28</v>
       </c>
-      <c r="O20" s="249"/>
-      <c r="P20" s="252" t="s">
+      <c r="O20" s="74"/>
+      <c r="P20" s="77" t="s">
         <v>20</v>
       </c>
-      <c r="Q20" s="253"/>
-      <c r="R20" s="240" t="s">
+      <c r="Q20" s="78"/>
+      <c r="R20" s="65" t="s">
         <v>21</v>
       </c>
-      <c r="S20" s="241"/>
+      <c r="S20" s="66"/>
       <c r="T20" s="6"/>
       <c r="U20" s="6"/>
       <c r="V20" s="6"/>
       <c r="W20" s="7"/>
     </row>
-    <row r="21" spans="10:23" ht="15.75" thickBot="1">
+    <row r="21" spans="1:23" ht="15.75" thickBot="1">
+      <c r="A21" s="5"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="7"/>
       <c r="J21" s="5"/>
       <c r="K21" s="6"/>
-      <c r="L21" s="246"/>
-      <c r="M21" s="247"/>
-      <c r="N21" s="250"/>
-      <c r="O21" s="251"/>
-      <c r="P21" s="254"/>
-      <c r="Q21" s="255"/>
-      <c r="R21" s="242"/>
-      <c r="S21" s="243"/>
+      <c r="L21" s="71"/>
+      <c r="M21" s="72"/>
+      <c r="N21" s="75"/>
+      <c r="O21" s="76"/>
+      <c r="P21" s="79"/>
+      <c r="Q21" s="80"/>
+      <c r="R21" s="67"/>
+      <c r="S21" s="68"/>
       <c r="T21" s="6"/>
       <c r="U21" s="6"/>
       <c r="V21" s="6"/>
       <c r="W21" s="7"/>
     </row>
-    <row r="22" spans="10:23">
+    <row r="22" spans="1:23">
+      <c r="A22" s="5"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="7"/>
       <c r="J22" s="5"/>
       <c r="K22" s="6"/>
-      <c r="L22" s="279" t="s">
+      <c r="L22" s="106" t="s">
         <v>27</v>
       </c>
-      <c r="M22" s="280"/>
-      <c r="N22" s="280"/>
-      <c r="O22" s="280"/>
-      <c r="P22" s="280"/>
-      <c r="Q22" s="280"/>
-      <c r="R22" s="280"/>
-      <c r="S22" s="281"/>
+      <c r="M22" s="107"/>
+      <c r="N22" s="107"/>
+      <c r="O22" s="107"/>
+      <c r="P22" s="107"/>
+      <c r="Q22" s="107"/>
+      <c r="R22" s="107"/>
+      <c r="S22" s="108"/>
       <c r="T22" s="6"/>
       <c r="U22" s="6"/>
       <c r="V22" s="6"/>
       <c r="W22" s="7"/>
     </row>
-    <row r="23" spans="10:23" ht="15.75" thickBot="1">
+    <row r="23" spans="1:23" ht="15.75" thickBot="1">
+      <c r="A23" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="C23" s="301" t="s">
+        <v>56</v>
+      </c>
+      <c r="D23" s="302"/>
+      <c r="E23" s="301" t="s">
+        <v>57</v>
+      </c>
+      <c r="F23" s="302"/>
+      <c r="G23" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="H23" s="7"/>
       <c r="J23" s="5"/>
       <c r="K23" s="6"/>
-      <c r="L23" s="282"/>
-      <c r="M23" s="283"/>
-      <c r="N23" s="283"/>
-      <c r="O23" s="283"/>
-      <c r="P23" s="283"/>
-      <c r="Q23" s="283"/>
-      <c r="R23" s="283"/>
-      <c r="S23" s="284"/>
+      <c r="L23" s="109"/>
+      <c r="M23" s="110"/>
+      <c r="N23" s="110"/>
+      <c r="O23" s="110"/>
+      <c r="P23" s="110"/>
+      <c r="Q23" s="110"/>
+      <c r="R23" s="110"/>
+      <c r="S23" s="111"/>
       <c r="T23" s="6"/>
       <c r="U23" s="6"/>
       <c r="V23" s="6"/>
       <c r="W23" s="7"/>
     </row>
-    <row r="24" spans="10:23">
+    <row r="24" spans="1:23">
+      <c r="A24" s="11"/>
+      <c r="B24" s="11"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="11"/>
+      <c r="H24" s="7"/>
       <c r="J24" s="5"/>
       <c r="K24" s="6"/>
       <c r="L24" s="6"/>
@@ -3274,7 +3441,15 @@
       <c r="V24" s="6"/>
       <c r="W24" s="7"/>
     </row>
-    <row r="25" spans="10:23" ht="15.75" thickBot="1">
+    <row r="25" spans="1:23" ht="15.75" thickBot="1">
+      <c r="A25" s="11"/>
+      <c r="B25" s="11"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="11"/>
+      <c r="H25" s="7"/>
       <c r="J25" s="8"/>
       <c r="K25" s="9"/>
       <c r="L25" s="9"/>
@@ -3290,753 +3465,909 @@
       <c r="V25" s="9"/>
       <c r="W25" s="10"/>
     </row>
-    <row r="27" spans="10:23" ht="15.75" thickBot="1"/>
-    <row r="28" spans="10:23">
-      <c r="J28" s="226" t="s">
+    <row r="26" spans="1:23">
+      <c r="A26" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B26" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="C26" s="301" t="s">
+        <v>61</v>
+      </c>
+      <c r="D26" s="304"/>
+      <c r="E26" s="303"/>
+      <c r="F26" s="11"/>
+      <c r="G26" s="11"/>
+      <c r="H26" s="7"/>
+    </row>
+    <row r="27" spans="1:23" ht="15.75" thickBot="1">
+      <c r="A27" s="11"/>
+      <c r="B27" s="11"/>
+      <c r="C27" s="11"/>
+      <c r="D27" s="11"/>
+      <c r="E27" s="11"/>
+      <c r="F27" s="11"/>
+      <c r="G27" s="11"/>
+      <c r="H27" s="7"/>
+    </row>
+    <row r="28" spans="1:23">
+      <c r="A28" s="11"/>
+      <c r="B28" s="11"/>
+      <c r="C28" s="11"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="11"/>
+      <c r="F28" s="11"/>
+      <c r="G28" s="11"/>
+      <c r="H28" s="7"/>
+      <c r="J28" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="K28" s="227"/>
-      <c r="L28" s="227"/>
-      <c r="M28" s="227"/>
-      <c r="N28" s="227"/>
-      <c r="O28" s="227"/>
-      <c r="P28" s="227"/>
-      <c r="Q28" s="227"/>
-      <c r="R28" s="227"/>
-      <c r="S28" s="227"/>
-      <c r="T28" s="227"/>
-      <c r="U28" s="227"/>
-      <c r="V28" s="227"/>
-      <c r="W28" s="228"/>
-    </row>
-    <row r="29" spans="10:23" ht="15.75" thickBot="1">
-      <c r="J29" s="229"/>
-      <c r="K29" s="230"/>
-      <c r="L29" s="230"/>
-      <c r="M29" s="230"/>
-      <c r="N29" s="230"/>
-      <c r="O29" s="230"/>
-      <c r="P29" s="230"/>
-      <c r="Q29" s="230"/>
-      <c r="R29" s="230"/>
-      <c r="S29" s="230"/>
-      <c r="T29" s="230"/>
-      <c r="U29" s="230"/>
-      <c r="V29" s="230"/>
-      <c r="W29" s="231"/>
-    </row>
-    <row r="30" spans="10:23" ht="15.75" thickBot="1"/>
-    <row r="31" spans="10:23">
-      <c r="J31" s="158" t="s">
+      <c r="K28" s="52"/>
+      <c r="L28" s="52"/>
+      <c r="M28" s="52"/>
+      <c r="N28" s="52"/>
+      <c r="O28" s="52"/>
+      <c r="P28" s="52"/>
+      <c r="Q28" s="52"/>
+      <c r="R28" s="52"/>
+      <c r="S28" s="52"/>
+      <c r="T28" s="52"/>
+      <c r="U28" s="52"/>
+      <c r="V28" s="52"/>
+      <c r="W28" s="53"/>
+    </row>
+    <row r="29" spans="1:23" ht="15.75" thickBot="1">
+      <c r="A29" s="11"/>
+      <c r="B29" s="11"/>
+      <c r="C29" s="11"/>
+      <c r="D29" s="11"/>
+      <c r="E29" s="11"/>
+      <c r="F29" s="11"/>
+      <c r="G29" s="11"/>
+      <c r="H29" s="7"/>
+      <c r="J29" s="54"/>
+      <c r="K29" s="55"/>
+      <c r="L29" s="55"/>
+      <c r="M29" s="55"/>
+      <c r="N29" s="55"/>
+      <c r="O29" s="55"/>
+      <c r="P29" s="55"/>
+      <c r="Q29" s="55"/>
+      <c r="R29" s="55"/>
+      <c r="S29" s="55"/>
+      <c r="T29" s="55"/>
+      <c r="U29" s="55"/>
+      <c r="V29" s="55"/>
+      <c r="W29" s="56"/>
+    </row>
+    <row r="30" spans="1:23" ht="15.75" thickBot="1">
+      <c r="A30" s="5"/>
+      <c r="B30" s="6"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="6"/>
+      <c r="H30" s="7"/>
+    </row>
+    <row r="31" spans="1:23">
+      <c r="A31" s="5"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="6"/>
+      <c r="H31" s="7"/>
+      <c r="J31" s="157" t="s">
         <v>35</v>
       </c>
-      <c r="K31" s="159"/>
-      <c r="L31" s="159"/>
-      <c r="M31" s="159"/>
-      <c r="N31" s="159"/>
-      <c r="O31" s="159"/>
-      <c r="P31" s="159"/>
-      <c r="Q31" s="159"/>
-      <c r="R31" s="159"/>
-      <c r="S31" s="159"/>
-      <c r="T31" s="159"/>
-      <c r="U31" s="159"/>
-      <c r="V31" s="159"/>
-      <c r="W31" s="160"/>
-    </row>
-    <row r="32" spans="10:23" ht="15.75" thickBot="1">
-      <c r="J32" s="161"/>
-      <c r="K32" s="162"/>
-      <c r="L32" s="162"/>
-      <c r="M32" s="162"/>
-      <c r="N32" s="162"/>
-      <c r="O32" s="162"/>
-      <c r="P32" s="162"/>
-      <c r="Q32" s="162"/>
-      <c r="R32" s="162"/>
-      <c r="S32" s="162"/>
-      <c r="T32" s="162"/>
-      <c r="U32" s="162"/>
-      <c r="V32" s="162"/>
-      <c r="W32" s="163"/>
+      <c r="K31" s="158"/>
+      <c r="L31" s="158"/>
+      <c r="M31" s="158"/>
+      <c r="N31" s="158"/>
+      <c r="O31" s="158"/>
+      <c r="P31" s="158"/>
+      <c r="Q31" s="158"/>
+      <c r="R31" s="158"/>
+      <c r="S31" s="158"/>
+      <c r="T31" s="158"/>
+      <c r="U31" s="158"/>
+      <c r="V31" s="158"/>
+      <c r="W31" s="159"/>
+    </row>
+    <row r="32" spans="1:23" ht="15.75" thickBot="1">
+      <c r="A32" s="8"/>
+      <c r="B32" s="9"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="9"/>
+      <c r="G32" s="9"/>
+      <c r="H32" s="10"/>
+      <c r="J32" s="160"/>
+      <c r="K32" s="161"/>
+      <c r="L32" s="161"/>
+      <c r="M32" s="161"/>
+      <c r="N32" s="161"/>
+      <c r="O32" s="161"/>
+      <c r="P32" s="161"/>
+      <c r="Q32" s="161"/>
+      <c r="R32" s="161"/>
+      <c r="S32" s="161"/>
+      <c r="T32" s="161"/>
+      <c r="U32" s="161"/>
+      <c r="V32" s="161"/>
+      <c r="W32" s="162"/>
     </row>
     <row r="33" spans="2:23" ht="15" customHeight="1">
       <c r="B33" s="6"/>
       <c r="C33" s="6"/>
       <c r="D33" s="6"/>
-      <c r="G33" s="45" t="s">
+      <c r="G33" s="216" t="s">
         <v>48</v>
       </c>
-      <c r="H33" s="61" t="s">
+      <c r="H33" s="232" t="s">
         <v>36</v>
       </c>
-      <c r="I33" s="62"/>
-      <c r="J33" s="57" t="s">
+      <c r="I33" s="231"/>
+      <c r="J33" s="227" t="s">
         <v>21</v>
       </c>
-      <c r="K33" s="58"/>
-      <c r="L33" s="164"/>
-      <c r="M33" s="165"/>
-      <c r="N33" s="165"/>
-      <c r="O33" s="165"/>
-      <c r="P33" s="165"/>
-      <c r="Q33" s="165"/>
-      <c r="R33" s="165"/>
-      <c r="S33" s="165"/>
-      <c r="T33" s="165"/>
-      <c r="U33" s="165"/>
-      <c r="V33" s="165"/>
-      <c r="W33" s="166"/>
+      <c r="K33" s="228"/>
+      <c r="L33" s="163"/>
+      <c r="M33" s="164"/>
+      <c r="N33" s="164"/>
+      <c r="O33" s="164"/>
+      <c r="P33" s="164"/>
+      <c r="Q33" s="164"/>
+      <c r="R33" s="164"/>
+      <c r="S33" s="164"/>
+      <c r="T33" s="164"/>
+      <c r="U33" s="164"/>
+      <c r="V33" s="164"/>
+      <c r="W33" s="165"/>
     </row>
     <row r="34" spans="2:23" ht="15" customHeight="1">
-      <c r="G34" s="46"/>
-      <c r="H34" s="63"/>
-      <c r="I34" s="64"/>
-      <c r="J34" s="59"/>
-      <c r="K34" s="60"/>
-      <c r="L34" s="167"/>
-      <c r="M34" s="168"/>
-      <c r="N34" s="168"/>
-      <c r="O34" s="168"/>
-      <c r="P34" s="168"/>
-      <c r="Q34" s="168"/>
-      <c r="R34" s="168"/>
-      <c r="S34" s="168"/>
-      <c r="T34" s="168"/>
-      <c r="U34" s="168"/>
-      <c r="V34" s="168"/>
-      <c r="W34" s="169"/>
+      <c r="G34" s="216"/>
+      <c r="H34" s="232"/>
+      <c r="I34" s="233"/>
+      <c r="J34" s="229"/>
+      <c r="K34" s="230"/>
+      <c r="L34" s="166"/>
+      <c r="M34" s="167"/>
+      <c r="N34" s="167"/>
+      <c r="O34" s="167"/>
+      <c r="P34" s="167"/>
+      <c r="Q34" s="167"/>
+      <c r="R34" s="167"/>
+      <c r="S34" s="167"/>
+      <c r="T34" s="167"/>
+      <c r="U34" s="167"/>
+      <c r="V34" s="167"/>
+      <c r="W34" s="168"/>
     </row>
     <row r="35" spans="2:23" ht="15" customHeight="1">
-      <c r="G35" s="46"/>
-      <c r="H35" s="63"/>
-      <c r="I35" s="64"/>
-      <c r="J35" s="59"/>
-      <c r="K35" s="60"/>
-      <c r="L35" s="167"/>
-      <c r="M35" s="168"/>
-      <c r="N35" s="168"/>
-      <c r="O35" s="168"/>
-      <c r="P35" s="168"/>
-      <c r="Q35" s="168"/>
-      <c r="R35" s="168"/>
-      <c r="S35" s="168"/>
-      <c r="T35" s="168"/>
-      <c r="U35" s="168"/>
-      <c r="V35" s="168"/>
-      <c r="W35" s="169"/>
+      <c r="G35" s="216"/>
+      <c r="H35" s="232"/>
+      <c r="I35" s="233"/>
+      <c r="J35" s="229"/>
+      <c r="K35" s="230"/>
+      <c r="L35" s="166"/>
+      <c r="M35" s="167"/>
+      <c r="N35" s="167"/>
+      <c r="O35" s="167"/>
+      <c r="P35" s="167"/>
+      <c r="Q35" s="167"/>
+      <c r="R35" s="167"/>
+      <c r="S35" s="167"/>
+      <c r="T35" s="167"/>
+      <c r="U35" s="167"/>
+      <c r="V35" s="167"/>
+      <c r="W35" s="168"/>
     </row>
     <row r="36" spans="2:23" ht="15" customHeight="1">
-      <c r="G36" s="46"/>
-      <c r="H36" s="63"/>
-      <c r="I36" s="64"/>
-      <c r="J36" s="59"/>
-      <c r="K36" s="60"/>
-      <c r="L36" s="167"/>
-      <c r="M36" s="168"/>
-      <c r="N36" s="168"/>
-      <c r="O36" s="168"/>
-      <c r="P36" s="168"/>
-      <c r="Q36" s="168"/>
-      <c r="R36" s="168"/>
-      <c r="S36" s="168"/>
-      <c r="T36" s="168"/>
-      <c r="U36" s="168"/>
-      <c r="V36" s="168"/>
-      <c r="W36" s="169"/>
+      <c r="G36" s="216"/>
+      <c r="H36" s="232"/>
+      <c r="I36" s="233"/>
+      <c r="J36" s="229"/>
+      <c r="K36" s="230"/>
+      <c r="L36" s="166"/>
+      <c r="M36" s="167"/>
+      <c r="N36" s="167"/>
+      <c r="O36" s="167"/>
+      <c r="P36" s="167"/>
+      <c r="Q36" s="167"/>
+      <c r="R36" s="167"/>
+      <c r="S36" s="167"/>
+      <c r="T36" s="167"/>
+      <c r="U36" s="167"/>
+      <c r="V36" s="167"/>
+      <c r="W36" s="168"/>
     </row>
     <row r="37" spans="2:23" ht="15" customHeight="1">
-      <c r="G37" s="46"/>
-      <c r="H37" s="63"/>
-      <c r="I37" s="64"/>
-      <c r="J37" s="59"/>
-      <c r="K37" s="60"/>
-      <c r="L37" s="167"/>
-      <c r="M37" s="168"/>
-      <c r="N37" s="168"/>
-      <c r="O37" s="168"/>
-      <c r="P37" s="168"/>
-      <c r="Q37" s="168"/>
-      <c r="R37" s="168"/>
-      <c r="S37" s="168"/>
-      <c r="T37" s="168"/>
-      <c r="U37" s="168"/>
-      <c r="V37" s="168"/>
-      <c r="W37" s="169"/>
+      <c r="G37" s="216"/>
+      <c r="H37" s="232"/>
+      <c r="I37" s="233"/>
+      <c r="J37" s="229"/>
+      <c r="K37" s="230"/>
+      <c r="L37" s="166"/>
+      <c r="M37" s="167"/>
+      <c r="N37" s="167"/>
+      <c r="O37" s="167"/>
+      <c r="P37" s="167"/>
+      <c r="Q37" s="167"/>
+      <c r="R37" s="167"/>
+      <c r="S37" s="167"/>
+      <c r="T37" s="167"/>
+      <c r="U37" s="167"/>
+      <c r="V37" s="167"/>
+      <c r="W37" s="168"/>
     </row>
     <row r="38" spans="2:23" ht="15" customHeight="1" thickBot="1">
-      <c r="G38" s="47"/>
-      <c r="H38" s="63"/>
-      <c r="I38" s="64"/>
-      <c r="J38" s="59"/>
-      <c r="K38" s="60"/>
-      <c r="L38" s="180"/>
-      <c r="M38" s="181"/>
-      <c r="N38" s="181"/>
-      <c r="O38" s="181"/>
-      <c r="P38" s="181"/>
-      <c r="Q38" s="181"/>
-      <c r="R38" s="181"/>
-      <c r="S38" s="181"/>
-      <c r="T38" s="181"/>
-      <c r="U38" s="181"/>
-      <c r="V38" s="181"/>
-      <c r="W38" s="182"/>
+      <c r="G38" s="217"/>
+      <c r="H38" s="232"/>
+      <c r="I38" s="233"/>
+      <c r="J38" s="229"/>
+      <c r="K38" s="230"/>
+      <c r="L38" s="201"/>
+      <c r="M38" s="202"/>
+      <c r="N38" s="202"/>
+      <c r="O38" s="202"/>
+      <c r="P38" s="202"/>
+      <c r="Q38" s="202"/>
+      <c r="R38" s="202"/>
+      <c r="S38" s="202"/>
+      <c r="T38" s="202"/>
+      <c r="U38" s="202"/>
+      <c r="V38" s="202"/>
+      <c r="W38" s="203"/>
     </row>
     <row r="39" spans="2:23" ht="15" customHeight="1">
-      <c r="H39" s="91" t="s">
+      <c r="H39" s="260" t="s">
         <v>41</v>
       </c>
-      <c r="I39" s="92"/>
-      <c r="J39" s="92"/>
-      <c r="K39" s="103" t="s">
+      <c r="I39" s="261"/>
+      <c r="J39" s="261"/>
+      <c r="K39" s="272" t="s">
         <v>42</v>
       </c>
-      <c r="L39" s="103"/>
-      <c r="M39" s="103"/>
-      <c r="N39" s="103"/>
-      <c r="O39" s="103"/>
-      <c r="P39" s="103"/>
-      <c r="Q39" s="103"/>
-      <c r="R39" s="103"/>
-      <c r="S39" s="103"/>
-      <c r="T39" s="103"/>
-      <c r="U39" s="103"/>
-      <c r="V39" s="103"/>
-      <c r="W39" s="104"/>
+      <c r="L39" s="272"/>
+      <c r="M39" s="272"/>
+      <c r="N39" s="272"/>
+      <c r="O39" s="272"/>
+      <c r="P39" s="272"/>
+      <c r="Q39" s="272"/>
+      <c r="R39" s="272"/>
+      <c r="S39" s="272"/>
+      <c r="T39" s="272"/>
+      <c r="U39" s="272"/>
+      <c r="V39" s="272"/>
+      <c r="W39" s="273"/>
     </row>
     <row r="40" spans="2:23" ht="15.75" customHeight="1" thickBot="1">
-      <c r="H40" s="93"/>
-      <c r="I40" s="94"/>
-      <c r="J40" s="94"/>
-      <c r="K40" s="105"/>
-      <c r="L40" s="105"/>
-      <c r="M40" s="105"/>
-      <c r="N40" s="105"/>
-      <c r="O40" s="105"/>
-      <c r="P40" s="105"/>
-      <c r="Q40" s="105"/>
-      <c r="R40" s="105"/>
-      <c r="S40" s="105"/>
-      <c r="T40" s="105"/>
-      <c r="U40" s="105"/>
-      <c r="V40" s="105"/>
-      <c r="W40" s="106"/>
+      <c r="H40" s="262"/>
+      <c r="I40" s="263"/>
+      <c r="J40" s="263"/>
+      <c r="K40" s="274"/>
+      <c r="L40" s="274"/>
+      <c r="M40" s="274"/>
+      <c r="N40" s="274"/>
+      <c r="O40" s="274"/>
+      <c r="P40" s="274"/>
+      <c r="Q40" s="274"/>
+      <c r="R40" s="274"/>
+      <c r="S40" s="274"/>
+      <c r="T40" s="274"/>
+      <c r="U40" s="274"/>
+      <c r="V40" s="274"/>
+      <c r="W40" s="275"/>
     </row>
     <row r="41" spans="2:23" ht="15" customHeight="1">
-      <c r="G41" s="54" t="s">
+      <c r="G41" s="224" t="s">
         <v>49</v>
       </c>
-      <c r="H41" s="79" t="s">
+      <c r="H41" s="248" t="s">
         <v>37</v>
       </c>
-      <c r="I41" s="80"/>
-      <c r="J41" s="65" t="s">
+      <c r="I41" s="249"/>
+      <c r="J41" s="234" t="s">
         <v>40</v>
       </c>
-      <c r="K41" s="66"/>
-      <c r="L41" s="140"/>
-      <c r="M41" s="141"/>
-      <c r="N41" s="141"/>
-      <c r="O41" s="141"/>
-      <c r="P41" s="141"/>
-      <c r="Q41" s="141"/>
-      <c r="R41" s="141"/>
-      <c r="S41" s="141"/>
-      <c r="T41" s="141"/>
-      <c r="U41" s="141"/>
-      <c r="V41" s="141"/>
-      <c r="W41" s="142"/>
+      <c r="K41" s="235"/>
+      <c r="L41" s="183"/>
+      <c r="M41" s="184"/>
+      <c r="N41" s="184"/>
+      <c r="O41" s="184"/>
+      <c r="P41" s="184"/>
+      <c r="Q41" s="184"/>
+      <c r="R41" s="184"/>
+      <c r="S41" s="184"/>
+      <c r="T41" s="184"/>
+      <c r="U41" s="184"/>
+      <c r="V41" s="184"/>
+      <c r="W41" s="185"/>
     </row>
     <row r="42" spans="2:23" ht="15" customHeight="1">
-      <c r="G42" s="55"/>
-      <c r="H42" s="81"/>
-      <c r="I42" s="82"/>
-      <c r="J42" s="67"/>
-      <c r="K42" s="68"/>
-      <c r="L42" s="174"/>
-      <c r="M42" s="175"/>
-      <c r="N42" s="175"/>
-      <c r="O42" s="175"/>
-      <c r="P42" s="175"/>
-      <c r="Q42" s="175"/>
-      <c r="R42" s="175"/>
-      <c r="S42" s="175"/>
-      <c r="T42" s="175"/>
-      <c r="U42" s="175"/>
-      <c r="V42" s="175"/>
-      <c r="W42" s="176"/>
+      <c r="G42" s="225"/>
+      <c r="H42" s="250"/>
+      <c r="I42" s="251"/>
+      <c r="J42" s="236"/>
+      <c r="K42" s="237"/>
+      <c r="L42" s="195"/>
+      <c r="M42" s="196"/>
+      <c r="N42" s="196"/>
+      <c r="O42" s="196"/>
+      <c r="P42" s="196"/>
+      <c r="Q42" s="196"/>
+      <c r="R42" s="196"/>
+      <c r="S42" s="196"/>
+      <c r="T42" s="196"/>
+      <c r="U42" s="196"/>
+      <c r="V42" s="196"/>
+      <c r="W42" s="197"/>
     </row>
     <row r="43" spans="2:23" ht="15" customHeight="1">
-      <c r="G43" s="55"/>
-      <c r="H43" s="81"/>
-      <c r="I43" s="82"/>
-      <c r="J43" s="67"/>
-      <c r="K43" s="68"/>
-      <c r="L43" s="174"/>
-      <c r="M43" s="175"/>
-      <c r="N43" s="175"/>
-      <c r="O43" s="175"/>
-      <c r="P43" s="175"/>
-      <c r="Q43" s="175"/>
-      <c r="R43" s="175"/>
-      <c r="S43" s="175"/>
-      <c r="T43" s="175"/>
-      <c r="U43" s="175"/>
-      <c r="V43" s="175"/>
-      <c r="W43" s="176"/>
+      <c r="G43" s="225"/>
+      <c r="H43" s="250"/>
+      <c r="I43" s="251"/>
+      <c r="J43" s="236"/>
+      <c r="K43" s="237"/>
+      <c r="L43" s="195"/>
+      <c r="M43" s="196"/>
+      <c r="N43" s="196"/>
+      <c r="O43" s="196"/>
+      <c r="P43" s="196"/>
+      <c r="Q43" s="196"/>
+      <c r="R43" s="196"/>
+      <c r="S43" s="196"/>
+      <c r="T43" s="196"/>
+      <c r="U43" s="196"/>
+      <c r="V43" s="196"/>
+      <c r="W43" s="197"/>
     </row>
     <row r="44" spans="2:23" ht="15" customHeight="1">
-      <c r="G44" s="55"/>
-      <c r="H44" s="81"/>
-      <c r="I44" s="82"/>
-      <c r="J44" s="67"/>
-      <c r="K44" s="68"/>
-      <c r="L44" s="174"/>
-      <c r="M44" s="175"/>
-      <c r="N44" s="175"/>
-      <c r="O44" s="175"/>
-      <c r="P44" s="175"/>
-      <c r="Q44" s="175"/>
-      <c r="R44" s="175"/>
-      <c r="S44" s="175"/>
-      <c r="T44" s="175"/>
-      <c r="U44" s="175"/>
-      <c r="V44" s="175"/>
-      <c r="W44" s="176"/>
+      <c r="G44" s="225"/>
+      <c r="H44" s="250"/>
+      <c r="I44" s="251"/>
+      <c r="J44" s="236"/>
+      <c r="K44" s="237"/>
+      <c r="L44" s="195"/>
+      <c r="M44" s="196"/>
+      <c r="N44" s="196"/>
+      <c r="O44" s="196"/>
+      <c r="P44" s="196"/>
+      <c r="Q44" s="196"/>
+      <c r="R44" s="196"/>
+      <c r="S44" s="196"/>
+      <c r="T44" s="196"/>
+      <c r="U44" s="196"/>
+      <c r="V44" s="196"/>
+      <c r="W44" s="197"/>
     </row>
     <row r="45" spans="2:23" ht="15" customHeight="1">
-      <c r="G45" s="55"/>
-      <c r="H45" s="81"/>
-      <c r="I45" s="82"/>
-      <c r="J45" s="67"/>
-      <c r="K45" s="68"/>
-      <c r="L45" s="174"/>
-      <c r="M45" s="175"/>
-      <c r="N45" s="175"/>
-      <c r="O45" s="175"/>
-      <c r="P45" s="175"/>
-      <c r="Q45" s="175"/>
-      <c r="R45" s="175"/>
-      <c r="S45" s="175"/>
-      <c r="T45" s="175"/>
-      <c r="U45" s="175"/>
-      <c r="V45" s="175"/>
-      <c r="W45" s="176"/>
+      <c r="G45" s="225"/>
+      <c r="H45" s="250"/>
+      <c r="I45" s="251"/>
+      <c r="J45" s="236"/>
+      <c r="K45" s="237"/>
+      <c r="L45" s="195"/>
+      <c r="M45" s="196"/>
+      <c r="N45" s="196"/>
+      <c r="O45" s="196"/>
+      <c r="P45" s="196"/>
+      <c r="Q45" s="196"/>
+      <c r="R45" s="196"/>
+      <c r="S45" s="196"/>
+      <c r="T45" s="196"/>
+      <c r="U45" s="196"/>
+      <c r="V45" s="196"/>
+      <c r="W45" s="197"/>
     </row>
     <row r="46" spans="2:23" ht="15" customHeight="1" thickBot="1">
-      <c r="G46" s="56"/>
-      <c r="H46" s="81"/>
-      <c r="I46" s="82"/>
-      <c r="J46" s="67"/>
-      <c r="K46" s="68"/>
-      <c r="L46" s="177"/>
-      <c r="M46" s="178"/>
-      <c r="N46" s="178"/>
-      <c r="O46" s="178"/>
-      <c r="P46" s="178"/>
-      <c r="Q46" s="178"/>
-      <c r="R46" s="178"/>
-      <c r="S46" s="178"/>
-      <c r="T46" s="178"/>
-      <c r="U46" s="178"/>
-      <c r="V46" s="178"/>
-      <c r="W46" s="179"/>
+      <c r="G46" s="226"/>
+      <c r="H46" s="250"/>
+      <c r="I46" s="251"/>
+      <c r="J46" s="236"/>
+      <c r="K46" s="237"/>
+      <c r="L46" s="198"/>
+      <c r="M46" s="199"/>
+      <c r="N46" s="199"/>
+      <c r="O46" s="199"/>
+      <c r="P46" s="199"/>
+      <c r="Q46" s="199"/>
+      <c r="R46" s="199"/>
+      <c r="S46" s="199"/>
+      <c r="T46" s="199"/>
+      <c r="U46" s="199"/>
+      <c r="V46" s="199"/>
+      <c r="W46" s="200"/>
     </row>
     <row r="47" spans="2:23" ht="15" customHeight="1">
-      <c r="H47" s="95" t="s">
+      <c r="H47" s="264" t="s">
         <v>41</v>
       </c>
-      <c r="I47" s="96"/>
-      <c r="J47" s="96"/>
-      <c r="K47" s="107" t="s">
+      <c r="I47" s="265"/>
+      <c r="J47" s="265"/>
+      <c r="K47" s="276" t="s">
         <v>43</v>
       </c>
-      <c r="L47" s="107"/>
-      <c r="M47" s="107"/>
-      <c r="N47" s="107"/>
-      <c r="O47" s="107"/>
-      <c r="P47" s="107"/>
-      <c r="Q47" s="107"/>
-      <c r="R47" s="107"/>
-      <c r="S47" s="107"/>
-      <c r="T47" s="107"/>
-      <c r="U47" s="107"/>
-      <c r="V47" s="107"/>
-      <c r="W47" s="108"/>
+      <c r="L47" s="276"/>
+      <c r="M47" s="276"/>
+      <c r="N47" s="276"/>
+      <c r="O47" s="276"/>
+      <c r="P47" s="276"/>
+      <c r="Q47" s="276"/>
+      <c r="R47" s="276"/>
+      <c r="S47" s="276"/>
+      <c r="T47" s="276"/>
+      <c r="U47" s="276"/>
+      <c r="V47" s="276"/>
+      <c r="W47" s="277"/>
     </row>
     <row r="48" spans="2:23" ht="15.75" customHeight="1" thickBot="1">
-      <c r="H48" s="97"/>
-      <c r="I48" s="98"/>
-      <c r="J48" s="98"/>
-      <c r="K48" s="109"/>
-      <c r="L48" s="109"/>
-      <c r="M48" s="109"/>
-      <c r="N48" s="109"/>
-      <c r="O48" s="109"/>
-      <c r="P48" s="109"/>
-      <c r="Q48" s="109"/>
-      <c r="R48" s="109"/>
-      <c r="S48" s="109"/>
-      <c r="T48" s="109"/>
-      <c r="U48" s="109"/>
-      <c r="V48" s="109"/>
-      <c r="W48" s="110"/>
+      <c r="H48" s="266"/>
+      <c r="I48" s="267"/>
+      <c r="J48" s="267"/>
+      <c r="K48" s="278"/>
+      <c r="L48" s="278"/>
+      <c r="M48" s="278"/>
+      <c r="N48" s="278"/>
+      <c r="O48" s="278"/>
+      <c r="P48" s="278"/>
+      <c r="Q48" s="278"/>
+      <c r="R48" s="278"/>
+      <c r="S48" s="278"/>
+      <c r="T48" s="278"/>
+      <c r="U48" s="278"/>
+      <c r="V48" s="278"/>
+      <c r="W48" s="279"/>
     </row>
     <row r="49" spans="7:23" ht="15" customHeight="1">
-      <c r="G49" s="51" t="s">
+      <c r="G49" s="221" t="s">
         <v>50</v>
       </c>
-      <c r="H49" s="83" t="s">
+      <c r="H49" s="252" t="s">
         <v>38</v>
       </c>
-      <c r="I49" s="84"/>
-      <c r="J49" s="69" t="s">
+      <c r="I49" s="253"/>
+      <c r="J49" s="238" t="s">
         <v>28</v>
       </c>
-      <c r="K49" s="70"/>
-      <c r="L49" s="149"/>
-      <c r="M49" s="150"/>
-      <c r="N49" s="150"/>
-      <c r="O49" s="150"/>
-      <c r="P49" s="150"/>
-      <c r="Q49" s="150"/>
-      <c r="R49" s="150"/>
-      <c r="S49" s="150"/>
-      <c r="T49" s="150"/>
-      <c r="U49" s="150"/>
-      <c r="V49" s="150"/>
-      <c r="W49" s="151"/>
+      <c r="K49" s="239"/>
+      <c r="L49" s="192"/>
+      <c r="M49" s="193"/>
+      <c r="N49" s="193"/>
+      <c r="O49" s="193"/>
+      <c r="P49" s="193"/>
+      <c r="Q49" s="193"/>
+      <c r="R49" s="193"/>
+      <c r="S49" s="193"/>
+      <c r="T49" s="193"/>
+      <c r="U49" s="193"/>
+      <c r="V49" s="193"/>
+      <c r="W49" s="194"/>
     </row>
     <row r="50" spans="7:23" ht="15" customHeight="1">
-      <c r="G50" s="52"/>
-      <c r="H50" s="85"/>
-      <c r="I50" s="86"/>
-      <c r="J50" s="71"/>
-      <c r="K50" s="72"/>
-      <c r="L50" s="143"/>
-      <c r="M50" s="144"/>
-      <c r="N50" s="144"/>
-      <c r="O50" s="144"/>
-      <c r="P50" s="144"/>
-      <c r="Q50" s="144"/>
-      <c r="R50" s="144"/>
-      <c r="S50" s="144"/>
-      <c r="T50" s="144"/>
-      <c r="U50" s="144"/>
-      <c r="V50" s="144"/>
-      <c r="W50" s="145"/>
+      <c r="G50" s="222"/>
+      <c r="H50" s="254"/>
+      <c r="I50" s="255"/>
+      <c r="J50" s="240"/>
+      <c r="K50" s="241"/>
+      <c r="L50" s="186"/>
+      <c r="M50" s="187"/>
+      <c r="N50" s="187"/>
+      <c r="O50" s="187"/>
+      <c r="P50" s="187"/>
+      <c r="Q50" s="187"/>
+      <c r="R50" s="187"/>
+      <c r="S50" s="187"/>
+      <c r="T50" s="187"/>
+      <c r="U50" s="187"/>
+      <c r="V50" s="187"/>
+      <c r="W50" s="188"/>
     </row>
     <row r="51" spans="7:23" ht="15" customHeight="1">
-      <c r="G51" s="52"/>
-      <c r="H51" s="85"/>
-      <c r="I51" s="86"/>
-      <c r="J51" s="71"/>
-      <c r="K51" s="72"/>
-      <c r="L51" s="143"/>
-      <c r="M51" s="144"/>
-      <c r="N51" s="144"/>
-      <c r="O51" s="144"/>
-      <c r="P51" s="144"/>
-      <c r="Q51" s="144"/>
-      <c r="R51" s="144"/>
-      <c r="S51" s="144"/>
-      <c r="T51" s="144"/>
-      <c r="U51" s="144"/>
-      <c r="V51" s="144"/>
-      <c r="W51" s="145"/>
+      <c r="G51" s="222"/>
+      <c r="H51" s="254"/>
+      <c r="I51" s="255"/>
+      <c r="J51" s="240"/>
+      <c r="K51" s="241"/>
+      <c r="L51" s="186"/>
+      <c r="M51" s="187"/>
+      <c r="N51" s="187"/>
+      <c r="O51" s="187"/>
+      <c r="P51" s="187"/>
+      <c r="Q51" s="187"/>
+      <c r="R51" s="187"/>
+      <c r="S51" s="187"/>
+      <c r="T51" s="187"/>
+      <c r="U51" s="187"/>
+      <c r="V51" s="187"/>
+      <c r="W51" s="188"/>
     </row>
     <row r="52" spans="7:23" ht="15" customHeight="1">
-      <c r="G52" s="52"/>
-      <c r="H52" s="85"/>
-      <c r="I52" s="86"/>
-      <c r="J52" s="71"/>
-      <c r="K52" s="72"/>
-      <c r="L52" s="143"/>
-      <c r="M52" s="144"/>
-      <c r="N52" s="144"/>
-      <c r="O52" s="144"/>
-      <c r="P52" s="144"/>
-      <c r="Q52" s="144"/>
-      <c r="R52" s="144"/>
-      <c r="S52" s="144"/>
-      <c r="T52" s="144"/>
-      <c r="U52" s="144"/>
-      <c r="V52" s="144"/>
-      <c r="W52" s="145"/>
+      <c r="G52" s="222"/>
+      <c r="H52" s="254"/>
+      <c r="I52" s="255"/>
+      <c r="J52" s="240"/>
+      <c r="K52" s="241"/>
+      <c r="L52" s="186"/>
+      <c r="M52" s="187"/>
+      <c r="N52" s="187"/>
+      <c r="O52" s="187"/>
+      <c r="P52" s="187"/>
+      <c r="Q52" s="187"/>
+      <c r="R52" s="187"/>
+      <c r="S52" s="187"/>
+      <c r="T52" s="187"/>
+      <c r="U52" s="187"/>
+      <c r="V52" s="187"/>
+      <c r="W52" s="188"/>
     </row>
     <row r="53" spans="7:23" ht="15" customHeight="1">
-      <c r="G53" s="52"/>
-      <c r="H53" s="85"/>
-      <c r="I53" s="86"/>
-      <c r="J53" s="71"/>
-      <c r="K53" s="72"/>
-      <c r="L53" s="143"/>
-      <c r="M53" s="144"/>
-      <c r="N53" s="144"/>
-      <c r="O53" s="144"/>
-      <c r="P53" s="144"/>
-      <c r="Q53" s="144"/>
-      <c r="R53" s="144"/>
-      <c r="S53" s="144"/>
-      <c r="T53" s="144"/>
-      <c r="U53" s="144"/>
-      <c r="V53" s="144"/>
-      <c r="W53" s="145"/>
+      <c r="G53" s="222"/>
+      <c r="H53" s="254"/>
+      <c r="I53" s="255"/>
+      <c r="J53" s="240"/>
+      <c r="K53" s="241"/>
+      <c r="L53" s="186"/>
+      <c r="M53" s="187"/>
+      <c r="N53" s="187"/>
+      <c r="O53" s="187"/>
+      <c r="P53" s="187"/>
+      <c r="Q53" s="187"/>
+      <c r="R53" s="187"/>
+      <c r="S53" s="187"/>
+      <c r="T53" s="187"/>
+      <c r="U53" s="187"/>
+      <c r="V53" s="187"/>
+      <c r="W53" s="188"/>
     </row>
     <row r="54" spans="7:23" ht="15" customHeight="1" thickBot="1">
-      <c r="G54" s="53"/>
-      <c r="H54" s="85"/>
-      <c r="I54" s="86"/>
-      <c r="J54" s="71"/>
-      <c r="K54" s="72"/>
-      <c r="L54" s="146"/>
-      <c r="M54" s="147"/>
-      <c r="N54" s="147"/>
-      <c r="O54" s="147"/>
-      <c r="P54" s="147"/>
-      <c r="Q54" s="147"/>
-      <c r="R54" s="147"/>
-      <c r="S54" s="147"/>
-      <c r="T54" s="147"/>
-      <c r="U54" s="147"/>
-      <c r="V54" s="147"/>
-      <c r="W54" s="148"/>
+      <c r="G54" s="223"/>
+      <c r="H54" s="254"/>
+      <c r="I54" s="255"/>
+      <c r="J54" s="240"/>
+      <c r="K54" s="241"/>
+      <c r="L54" s="189"/>
+      <c r="M54" s="190"/>
+      <c r="N54" s="190"/>
+      <c r="O54" s="190"/>
+      <c r="P54" s="190"/>
+      <c r="Q54" s="190"/>
+      <c r="R54" s="190"/>
+      <c r="S54" s="190"/>
+      <c r="T54" s="190"/>
+      <c r="U54" s="190"/>
+      <c r="V54" s="190"/>
+      <c r="W54" s="191"/>
     </row>
     <row r="55" spans="7:23" ht="15" customHeight="1">
-      <c r="H55" s="99" t="s">
+      <c r="H55" s="268" t="s">
         <v>41</v>
       </c>
-      <c r="I55" s="100"/>
-      <c r="J55" s="100"/>
-      <c r="K55" s="111" t="s">
+      <c r="I55" s="269"/>
+      <c r="J55" s="269"/>
+      <c r="K55" s="280" t="s">
         <v>44</v>
       </c>
-      <c r="L55" s="111"/>
-      <c r="M55" s="111"/>
-      <c r="N55" s="111"/>
-      <c r="O55" s="111"/>
-      <c r="P55" s="111"/>
-      <c r="Q55" s="111"/>
-      <c r="R55" s="111"/>
-      <c r="S55" s="111"/>
-      <c r="T55" s="111"/>
-      <c r="U55" s="111"/>
-      <c r="V55" s="111"/>
-      <c r="W55" s="112"/>
+      <c r="L55" s="280"/>
+      <c r="M55" s="280"/>
+      <c r="N55" s="280"/>
+      <c r="O55" s="280"/>
+      <c r="P55" s="280"/>
+      <c r="Q55" s="280"/>
+      <c r="R55" s="280"/>
+      <c r="S55" s="280"/>
+      <c r="T55" s="280"/>
+      <c r="U55" s="280"/>
+      <c r="V55" s="280"/>
+      <c r="W55" s="281"/>
     </row>
     <row r="56" spans="7:23" ht="15.75" customHeight="1" thickBot="1">
-      <c r="H56" s="101"/>
-      <c r="I56" s="102"/>
-      <c r="J56" s="102"/>
-      <c r="K56" s="113"/>
-      <c r="L56" s="113"/>
-      <c r="M56" s="113"/>
-      <c r="N56" s="113"/>
-      <c r="O56" s="113"/>
-      <c r="P56" s="113"/>
-      <c r="Q56" s="113"/>
-      <c r="R56" s="113"/>
-      <c r="S56" s="113"/>
-      <c r="T56" s="113"/>
-      <c r="U56" s="113"/>
-      <c r="V56" s="113"/>
-      <c r="W56" s="114"/>
+      <c r="H56" s="270"/>
+      <c r="I56" s="271"/>
+      <c r="J56" s="271"/>
+      <c r="K56" s="282"/>
+      <c r="L56" s="282"/>
+      <c r="M56" s="282"/>
+      <c r="N56" s="282"/>
+      <c r="O56" s="282"/>
+      <c r="P56" s="282"/>
+      <c r="Q56" s="282"/>
+      <c r="R56" s="282"/>
+      <c r="S56" s="282"/>
+      <c r="T56" s="282"/>
+      <c r="U56" s="282"/>
+      <c r="V56" s="282"/>
+      <c r="W56" s="283"/>
     </row>
     <row r="57" spans="7:23" ht="15" customHeight="1">
-      <c r="G57" s="48" t="s">
+      <c r="G57" s="218" t="s">
         <v>51</v>
       </c>
-      <c r="H57" s="87" t="s">
+      <c r="H57" s="256" t="s">
         <v>39</v>
       </c>
-      <c r="I57" s="88"/>
-      <c r="J57" s="73" t="s">
+      <c r="I57" s="257"/>
+      <c r="J57" s="242" t="s">
         <v>45</v>
       </c>
-      <c r="K57" s="74"/>
-      <c r="L57" s="134"/>
-      <c r="M57" s="135"/>
-      <c r="N57" s="135"/>
-      <c r="O57" s="135"/>
-      <c r="P57" s="135"/>
-      <c r="Q57" s="135"/>
-      <c r="R57" s="135"/>
-      <c r="S57" s="135"/>
-      <c r="T57" s="135"/>
-      <c r="U57" s="135"/>
-      <c r="V57" s="135"/>
-      <c r="W57" s="136"/>
+      <c r="K57" s="243"/>
+      <c r="L57" s="177"/>
+      <c r="M57" s="178"/>
+      <c r="N57" s="178"/>
+      <c r="O57" s="178"/>
+      <c r="P57" s="178"/>
+      <c r="Q57" s="178"/>
+      <c r="R57" s="178"/>
+      <c r="S57" s="178"/>
+      <c r="T57" s="178"/>
+      <c r="U57" s="178"/>
+      <c r="V57" s="178"/>
+      <c r="W57" s="179"/>
     </row>
     <row r="58" spans="7:23" ht="15" customHeight="1">
-      <c r="G58" s="49"/>
-      <c r="H58" s="89"/>
-      <c r="I58" s="90"/>
-      <c r="J58" s="75"/>
-      <c r="K58" s="76"/>
-      <c r="L58" s="137"/>
-      <c r="M58" s="138"/>
-      <c r="N58" s="138"/>
-      <c r="O58" s="138"/>
-      <c r="P58" s="138"/>
-      <c r="Q58" s="138"/>
-      <c r="R58" s="138"/>
-      <c r="S58" s="138"/>
-      <c r="T58" s="138"/>
-      <c r="U58" s="138"/>
-      <c r="V58" s="138"/>
-      <c r="W58" s="139"/>
+      <c r="G58" s="219"/>
+      <c r="H58" s="258"/>
+      <c r="I58" s="259"/>
+      <c r="J58" s="244"/>
+      <c r="K58" s="245"/>
+      <c r="L58" s="180"/>
+      <c r="M58" s="181"/>
+      <c r="N58" s="181"/>
+      <c r="O58" s="181"/>
+      <c r="P58" s="181"/>
+      <c r="Q58" s="181"/>
+      <c r="R58" s="181"/>
+      <c r="S58" s="181"/>
+      <c r="T58" s="181"/>
+      <c r="U58" s="181"/>
+      <c r="V58" s="181"/>
+      <c r="W58" s="182"/>
     </row>
     <row r="59" spans="7:23" ht="15" customHeight="1">
-      <c r="G59" s="49"/>
-      <c r="H59" s="89"/>
-      <c r="I59" s="90"/>
-      <c r="J59" s="75"/>
-      <c r="K59" s="76"/>
-      <c r="L59" s="137"/>
-      <c r="M59" s="138"/>
-      <c r="N59" s="138"/>
-      <c r="O59" s="138"/>
-      <c r="P59" s="138"/>
-      <c r="Q59" s="138"/>
-      <c r="R59" s="138"/>
-      <c r="S59" s="138"/>
-      <c r="T59" s="138"/>
-      <c r="U59" s="138"/>
-      <c r="V59" s="138"/>
-      <c r="W59" s="139"/>
+      <c r="G59" s="219"/>
+      <c r="H59" s="258"/>
+      <c r="I59" s="259"/>
+      <c r="J59" s="244"/>
+      <c r="K59" s="245"/>
+      <c r="L59" s="180"/>
+      <c r="M59" s="181"/>
+      <c r="N59" s="181"/>
+      <c r="O59" s="181"/>
+      <c r="P59" s="181"/>
+      <c r="Q59" s="181"/>
+      <c r="R59" s="181"/>
+      <c r="S59" s="181"/>
+      <c r="T59" s="181"/>
+      <c r="U59" s="181"/>
+      <c r="V59" s="181"/>
+      <c r="W59" s="182"/>
     </row>
     <row r="60" spans="7:23" ht="15" customHeight="1">
-      <c r="G60" s="49"/>
-      <c r="H60" s="89"/>
-      <c r="I60" s="90"/>
-      <c r="J60" s="75"/>
-      <c r="K60" s="76"/>
-      <c r="L60" s="137"/>
-      <c r="M60" s="138"/>
-      <c r="N60" s="138"/>
-      <c r="O60" s="138"/>
-      <c r="P60" s="138"/>
-      <c r="Q60" s="138"/>
-      <c r="R60" s="138"/>
-      <c r="S60" s="138"/>
-      <c r="T60" s="138"/>
-      <c r="U60" s="138"/>
-      <c r="V60" s="138"/>
-      <c r="W60" s="139"/>
+      <c r="G60" s="219"/>
+      <c r="H60" s="258"/>
+      <c r="I60" s="259"/>
+      <c r="J60" s="244"/>
+      <c r="K60" s="245"/>
+      <c r="L60" s="180"/>
+      <c r="M60" s="181"/>
+      <c r="N60" s="181"/>
+      <c r="O60" s="181"/>
+      <c r="P60" s="181"/>
+      <c r="Q60" s="181"/>
+      <c r="R60" s="181"/>
+      <c r="S60" s="181"/>
+      <c r="T60" s="181"/>
+      <c r="U60" s="181"/>
+      <c r="V60" s="181"/>
+      <c r="W60" s="182"/>
     </row>
     <row r="61" spans="7:23" ht="15" customHeight="1">
-      <c r="G61" s="49"/>
-      <c r="H61" s="89"/>
-      <c r="I61" s="90"/>
-      <c r="J61" s="75"/>
-      <c r="K61" s="76"/>
-      <c r="L61" s="137"/>
-      <c r="M61" s="138"/>
-      <c r="N61" s="138"/>
-      <c r="O61" s="138"/>
-      <c r="P61" s="138"/>
-      <c r="Q61" s="138"/>
-      <c r="R61" s="138"/>
-      <c r="S61" s="138"/>
-      <c r="T61" s="138"/>
-      <c r="U61" s="138"/>
-      <c r="V61" s="138"/>
-      <c r="W61" s="139"/>
+      <c r="G61" s="219"/>
+      <c r="H61" s="258"/>
+      <c r="I61" s="259"/>
+      <c r="J61" s="244"/>
+      <c r="K61" s="245"/>
+      <c r="L61" s="180"/>
+      <c r="M61" s="181"/>
+      <c r="N61" s="181"/>
+      <c r="O61" s="181"/>
+      <c r="P61" s="181"/>
+      <c r="Q61" s="181"/>
+      <c r="R61" s="181"/>
+      <c r="S61" s="181"/>
+      <c r="T61" s="181"/>
+      <c r="U61" s="181"/>
+      <c r="V61" s="181"/>
+      <c r="W61" s="182"/>
     </row>
     <row r="62" spans="7:23" ht="15" customHeight="1" thickBot="1">
-      <c r="G62" s="50"/>
-      <c r="H62" s="89"/>
-      <c r="I62" s="90"/>
-      <c r="J62" s="77"/>
-      <c r="K62" s="78"/>
-      <c r="L62" s="115"/>
-      <c r="M62" s="116"/>
-      <c r="N62" s="116"/>
-      <c r="O62" s="116"/>
-      <c r="P62" s="116"/>
-      <c r="Q62" s="116"/>
-      <c r="R62" s="116"/>
-      <c r="S62" s="116"/>
-      <c r="T62" s="116"/>
-      <c r="U62" s="116"/>
-      <c r="V62" s="116"/>
-      <c r="W62" s="117"/>
+      <c r="G62" s="220"/>
+      <c r="H62" s="258"/>
+      <c r="I62" s="259"/>
+      <c r="J62" s="246"/>
+      <c r="K62" s="247"/>
+      <c r="L62" s="284"/>
+      <c r="M62" s="285"/>
+      <c r="N62" s="285"/>
+      <c r="O62" s="285"/>
+      <c r="P62" s="285"/>
+      <c r="Q62" s="285"/>
+      <c r="R62" s="285"/>
+      <c r="S62" s="285"/>
+      <c r="T62" s="285"/>
+      <c r="U62" s="285"/>
+      <c r="V62" s="285"/>
+      <c r="W62" s="286"/>
     </row>
     <row r="63" spans="7:23" ht="15" customHeight="1">
-      <c r="H63" s="152" t="s">
+      <c r="H63" s="287" t="s">
         <v>41</v>
       </c>
-      <c r="I63" s="153"/>
-      <c r="J63" s="153"/>
-      <c r="K63" s="40" t="s">
+      <c r="I63" s="288"/>
+      <c r="J63" s="288"/>
+      <c r="K63" s="211" t="s">
         <v>46</v>
       </c>
-      <c r="L63" s="40"/>
-      <c r="M63" s="40"/>
-      <c r="N63" s="40"/>
-      <c r="O63" s="40"/>
-      <c r="P63" s="40"/>
-      <c r="Q63" s="40"/>
-      <c r="R63" s="40"/>
-      <c r="S63" s="40"/>
-      <c r="T63" s="40"/>
-      <c r="U63" s="40"/>
-      <c r="V63" s="40"/>
-      <c r="W63" s="41"/>
+      <c r="L63" s="211"/>
+      <c r="M63" s="211"/>
+      <c r="N63" s="211"/>
+      <c r="O63" s="211"/>
+      <c r="P63" s="211"/>
+      <c r="Q63" s="211"/>
+      <c r="R63" s="211"/>
+      <c r="S63" s="211"/>
+      <c r="T63" s="211"/>
+      <c r="U63" s="211"/>
+      <c r="V63" s="211"/>
+      <c r="W63" s="212"/>
     </row>
     <row r="64" spans="7:23" ht="15.75" customHeight="1" thickBot="1">
-      <c r="H64" s="154"/>
-      <c r="I64" s="155"/>
-      <c r="J64" s="155"/>
-      <c r="K64" s="43"/>
-      <c r="L64" s="43"/>
-      <c r="M64" s="43"/>
-      <c r="N64" s="43"/>
-      <c r="O64" s="43"/>
-      <c r="P64" s="43"/>
-      <c r="Q64" s="43"/>
-      <c r="R64" s="43"/>
-      <c r="S64" s="43"/>
-      <c r="T64" s="43"/>
-      <c r="U64" s="43"/>
-      <c r="V64" s="43"/>
-      <c r="W64" s="44"/>
+      <c r="H64" s="289"/>
+      <c r="I64" s="290"/>
+      <c r="J64" s="290"/>
+      <c r="K64" s="214"/>
+      <c r="L64" s="214"/>
+      <c r="M64" s="214"/>
+      <c r="N64" s="214"/>
+      <c r="O64" s="214"/>
+      <c r="P64" s="214"/>
+      <c r="Q64" s="214"/>
+      <c r="R64" s="214"/>
+      <c r="S64" s="214"/>
+      <c r="T64" s="214"/>
+      <c r="U64" s="214"/>
+      <c r="V64" s="214"/>
+      <c r="W64" s="215"/>
     </row>
     <row r="65" spans="11:23">
-      <c r="K65" s="39" t="s">
+      <c r="K65" s="210" t="s">
         <v>47</v>
       </c>
-      <c r="L65" s="40"/>
-      <c r="M65" s="40"/>
-      <c r="N65" s="40"/>
-      <c r="O65" s="40"/>
-      <c r="P65" s="40"/>
-      <c r="Q65" s="40"/>
-      <c r="R65" s="40"/>
-      <c r="S65" s="40"/>
-      <c r="T65" s="40"/>
-      <c r="U65" s="40"/>
-      <c r="V65" s="40"/>
-      <c r="W65" s="41"/>
+      <c r="L65" s="211"/>
+      <c r="M65" s="211"/>
+      <c r="N65" s="211"/>
+      <c r="O65" s="211"/>
+      <c r="P65" s="211"/>
+      <c r="Q65" s="211"/>
+      <c r="R65" s="211"/>
+      <c r="S65" s="211"/>
+      <c r="T65" s="211"/>
+      <c r="U65" s="211"/>
+      <c r="V65" s="211"/>
+      <c r="W65" s="212"/>
     </row>
     <row r="66" spans="11:23" ht="15.75" thickBot="1">
-      <c r="K66" s="42"/>
-      <c r="L66" s="43"/>
-      <c r="M66" s="43"/>
-      <c r="N66" s="43"/>
-      <c r="O66" s="43"/>
-      <c r="P66" s="43"/>
-      <c r="Q66" s="43"/>
-      <c r="R66" s="43"/>
-      <c r="S66" s="43"/>
-      <c r="T66" s="43"/>
-      <c r="U66" s="43"/>
-      <c r="V66" s="43"/>
-      <c r="W66" s="44"/>
+      <c r="K66" s="213"/>
+      <c r="L66" s="214"/>
+      <c r="M66" s="214"/>
+      <c r="N66" s="214"/>
+      <c r="O66" s="214"/>
+      <c r="P66" s="214"/>
+      <c r="Q66" s="214"/>
+      <c r="R66" s="214"/>
+      <c r="S66" s="214"/>
+      <c r="T66" s="214"/>
+      <c r="U66" s="214"/>
+      <c r="V66" s="214"/>
+      <c r="W66" s="215"/>
     </row>
   </sheetData>
-  <mergeCells count="109">
+  <mergeCells count="114">
+    <mergeCell ref="B19:C20"/>
+    <mergeCell ref="E19:G20"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="K65:W66"/>
+    <mergeCell ref="G33:G38"/>
+    <mergeCell ref="G57:G62"/>
+    <mergeCell ref="G49:G54"/>
+    <mergeCell ref="G41:G46"/>
+    <mergeCell ref="J33:K38"/>
+    <mergeCell ref="H33:I38"/>
+    <mergeCell ref="J41:K46"/>
+    <mergeCell ref="J49:K54"/>
+    <mergeCell ref="J57:K62"/>
+    <mergeCell ref="H41:I46"/>
+    <mergeCell ref="H49:I54"/>
+    <mergeCell ref="H57:I62"/>
+    <mergeCell ref="H39:J40"/>
+    <mergeCell ref="H47:J48"/>
+    <mergeCell ref="H55:J56"/>
+    <mergeCell ref="K39:W40"/>
+    <mergeCell ref="K47:W48"/>
+    <mergeCell ref="K55:W56"/>
+    <mergeCell ref="L62:W62"/>
+    <mergeCell ref="H63:J64"/>
+    <mergeCell ref="K63:W64"/>
+    <mergeCell ref="L37:W37"/>
+    <mergeCell ref="L38:W38"/>
+    <mergeCell ref="N7:O7"/>
+    <mergeCell ref="N8:O8"/>
+    <mergeCell ref="N9:O9"/>
+    <mergeCell ref="N10:O10"/>
+    <mergeCell ref="N11:O11"/>
+    <mergeCell ref="N12:O12"/>
+    <mergeCell ref="N13:O13"/>
+    <mergeCell ref="N14:O14"/>
+    <mergeCell ref="N15:O15"/>
+    <mergeCell ref="L57:W57"/>
+    <mergeCell ref="L58:W58"/>
+    <mergeCell ref="L59:W59"/>
+    <mergeCell ref="L60:W60"/>
+    <mergeCell ref="L61:W61"/>
+    <mergeCell ref="L41:W41"/>
+    <mergeCell ref="L52:W52"/>
+    <mergeCell ref="L53:W53"/>
+    <mergeCell ref="L54:W54"/>
+    <mergeCell ref="L49:W49"/>
+    <mergeCell ref="L50:W50"/>
+    <mergeCell ref="L51:W51"/>
+    <mergeCell ref="L42:W42"/>
+    <mergeCell ref="L43:W43"/>
+    <mergeCell ref="L44:W44"/>
+    <mergeCell ref="L45:W45"/>
+    <mergeCell ref="L46:W46"/>
+    <mergeCell ref="J31:W32"/>
+    <mergeCell ref="L33:W33"/>
+    <mergeCell ref="L34:W34"/>
+    <mergeCell ref="L35:W35"/>
+    <mergeCell ref="L36:W36"/>
+    <mergeCell ref="M17:M18"/>
+    <mergeCell ref="P18:Q18"/>
+    <mergeCell ref="P16:Q16"/>
+    <mergeCell ref="P17:Q17"/>
+    <mergeCell ref="N16:O16"/>
+    <mergeCell ref="N17:O17"/>
+    <mergeCell ref="N18:O18"/>
+    <mergeCell ref="M13:M14"/>
+    <mergeCell ref="M15:M16"/>
+    <mergeCell ref="P13:Q13"/>
+    <mergeCell ref="P14:Q14"/>
+    <mergeCell ref="R7:S7"/>
+    <mergeCell ref="K7:L10"/>
+    <mergeCell ref="M7:M10"/>
+    <mergeCell ref="M11:M12"/>
+    <mergeCell ref="K11:L12"/>
+    <mergeCell ref="R13:S13"/>
+    <mergeCell ref="R14:S14"/>
+    <mergeCell ref="P8:Q8"/>
+    <mergeCell ref="P9:Q9"/>
+    <mergeCell ref="P10:Q10"/>
+    <mergeCell ref="P11:Q11"/>
+    <mergeCell ref="P12:Q12"/>
+    <mergeCell ref="R8:S8"/>
+    <mergeCell ref="R9:S9"/>
+    <mergeCell ref="R10:S10"/>
+    <mergeCell ref="R11:S11"/>
+    <mergeCell ref="R12:S12"/>
+    <mergeCell ref="R15:S15"/>
+    <mergeCell ref="R16:S16"/>
     <mergeCell ref="R6:S6"/>
     <mergeCell ref="P6:Q6"/>
     <mergeCell ref="A14:B14"/>
@@ -4061,91 +4392,6 @@
     <mergeCell ref="R17:S17"/>
     <mergeCell ref="R18:S18"/>
     <mergeCell ref="P15:Q15"/>
-    <mergeCell ref="M13:M14"/>
-    <mergeCell ref="M15:M16"/>
-    <mergeCell ref="P13:Q13"/>
-    <mergeCell ref="P14:Q14"/>
-    <mergeCell ref="R7:S7"/>
-    <mergeCell ref="K7:L10"/>
-    <mergeCell ref="M7:M10"/>
-    <mergeCell ref="M11:M12"/>
-    <mergeCell ref="K11:L12"/>
-    <mergeCell ref="R13:S13"/>
-    <mergeCell ref="R14:S14"/>
-    <mergeCell ref="P8:Q8"/>
-    <mergeCell ref="P9:Q9"/>
-    <mergeCell ref="P10:Q10"/>
-    <mergeCell ref="P11:Q11"/>
-    <mergeCell ref="P12:Q12"/>
-    <mergeCell ref="R8:S8"/>
-    <mergeCell ref="R9:S9"/>
-    <mergeCell ref="R10:S10"/>
-    <mergeCell ref="R11:S11"/>
-    <mergeCell ref="R12:S12"/>
-    <mergeCell ref="R15:S15"/>
-    <mergeCell ref="R16:S16"/>
-    <mergeCell ref="J31:W32"/>
-    <mergeCell ref="L33:W33"/>
-    <mergeCell ref="L34:W34"/>
-    <mergeCell ref="L35:W35"/>
-    <mergeCell ref="L36:W36"/>
-    <mergeCell ref="M17:M18"/>
-    <mergeCell ref="P18:Q18"/>
-    <mergeCell ref="P16:Q16"/>
-    <mergeCell ref="P17:Q17"/>
-    <mergeCell ref="N16:O16"/>
-    <mergeCell ref="N17:O17"/>
-    <mergeCell ref="N18:O18"/>
-    <mergeCell ref="L57:W57"/>
-    <mergeCell ref="L58:W58"/>
-    <mergeCell ref="L59:W59"/>
-    <mergeCell ref="L60:W60"/>
-    <mergeCell ref="L61:W61"/>
-    <mergeCell ref="L41:W41"/>
-    <mergeCell ref="L52:W52"/>
-    <mergeCell ref="L53:W53"/>
-    <mergeCell ref="L54:W54"/>
-    <mergeCell ref="L49:W49"/>
-    <mergeCell ref="L50:W50"/>
-    <mergeCell ref="L51:W51"/>
-    <mergeCell ref="L42:W42"/>
-    <mergeCell ref="L43:W43"/>
-    <mergeCell ref="L44:W44"/>
-    <mergeCell ref="L45:W45"/>
-    <mergeCell ref="L46:W46"/>
-    <mergeCell ref="L37:W37"/>
-    <mergeCell ref="L38:W38"/>
-    <mergeCell ref="N7:O7"/>
-    <mergeCell ref="N8:O8"/>
-    <mergeCell ref="N9:O9"/>
-    <mergeCell ref="N10:O10"/>
-    <mergeCell ref="N11:O11"/>
-    <mergeCell ref="N12:O12"/>
-    <mergeCell ref="N13:O13"/>
-    <mergeCell ref="N14:O14"/>
-    <mergeCell ref="N15:O15"/>
-    <mergeCell ref="K65:W66"/>
-    <mergeCell ref="G33:G38"/>
-    <mergeCell ref="G57:G62"/>
-    <mergeCell ref="G49:G54"/>
-    <mergeCell ref="G41:G46"/>
-    <mergeCell ref="J33:K38"/>
-    <mergeCell ref="H33:I38"/>
-    <mergeCell ref="J41:K46"/>
-    <mergeCell ref="J49:K54"/>
-    <mergeCell ref="J57:K62"/>
-    <mergeCell ref="H41:I46"/>
-    <mergeCell ref="H49:I54"/>
-    <mergeCell ref="H57:I62"/>
-    <mergeCell ref="H39:J40"/>
-    <mergeCell ref="H47:J48"/>
-    <mergeCell ref="H55:J56"/>
-    <mergeCell ref="K39:W40"/>
-    <mergeCell ref="K47:W48"/>
-    <mergeCell ref="K55:W56"/>
-    <mergeCell ref="L62:W62"/>
-    <mergeCell ref="H63:J64"/>
-    <mergeCell ref="K63:W64"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>